<commit_message>
keine Ahnung was neu
</commit_message>
<xml_diff>
--- a/divingComputer/diveTableMeters.xlsx
+++ b/divingComputer/diveTableMeters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jenny\Documents\Demonstratoren\divingComputer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{39AE981C-94B9-407E-A616-0AF861A0A093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{643AB6C3-0DC7-4F59-A163-C80379DC66BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{25DEC11B-994E-4242-B1D9-DE066B49018D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="2" xr2:uid="{25DEC11B-994E-4242-B1D9-DE066B49018D}"/>
   </bookViews>
   <sheets>
     <sheet name="feet" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="32">
   <si>
     <t>A</t>
   </si>
@@ -211,6 +211,40 @@
       <t xml:space="preserve"> pressure group at the end of surface intervall</t>
     </r>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Pressure group</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>depth in meter</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -271,7 +305,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -308,6 +342,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="15"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -429,7 +469,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -506,6 +546,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -3147,8 +3188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4850419-6222-4679-9F7A-92E5967F322E}">
   <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3158,7 +3199,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="16.8" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B1">
         <f>feet!B1/3.28084</f>
@@ -3246,6 +3287,9 @@
       <c r="L2">
         <v>3</v>
       </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -3287,9 +3331,6 @@
       <c r="M3">
         <v>4</v>
       </c>
-      <c r="O3" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -3407,6 +3448,9 @@
       <c r="K6">
         <v>8</v>
       </c>
+      <c r="L6">
+        <v>7</v>
+      </c>
       <c r="M6">
         <v>7</v>
       </c>
@@ -3521,6 +3565,9 @@
       <c r="J9">
         <v>12</v>
       </c>
+      <c r="K9">
+        <v>10</v>
+      </c>
       <c r="L9" s="3">
         <v>10</v>
       </c>
@@ -3559,9 +3606,7 @@
       <c r="K10">
         <v>11</v>
       </c>
-      <c r="O10" s="3" t="s">
-        <v>28</v>
-      </c>
+      <c r="O10" s="28"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -3590,6 +3635,9 @@
       </c>
       <c r="I11">
         <v>15</v>
+      </c>
+      <c r="J11">
+        <v>14</v>
       </c>
       <c r="K11">
         <v>12</v>
@@ -7028,9 +7076,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BB05363-7C20-4811-B333-E0099FBE82F3}">
   <dimension ref="A1:AA23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>